<commit_message>
Updated data feeds except mine netback and interim
</commit_message>
<xml_diff>
--- a/DataFeeds/BrazilCFR.xlsx
+++ b/DataFeeds/BrazilCFR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAFC48CB-C56C-4981-882C-938C72487621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE4D80-C13A-4C43-8A61-CB10B4F8A8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{8A4C0F15-AD97-40A7-9824-0E46FEA19653}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8A4C0F15-AD97-40A7-9824-0E46FEA19653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -93,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,15 +102,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0731233C-0420-4FB5-BC73-AB9A7C487093}">
-  <dimension ref="A1:B176"/>
+  <dimension ref="A1:B184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177:XFD181"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176:A184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -454,7 +469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>39448</v>
       </c>
@@ -462,7 +477,7 @@
         <v>427.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>39479</v>
       </c>
@@ -470,7 +485,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>39508</v>
       </c>
@@ -478,7 +493,7 @@
         <v>512.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>39539</v>
       </c>
@@ -486,7 +501,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>39569</v>
       </c>
@@ -494,7 +509,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>39600</v>
       </c>
@@ -502,7 +517,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>39630</v>
       </c>
@@ -510,7 +525,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>39661</v>
       </c>
@@ -518,7 +533,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>39692</v>
       </c>
@@ -526,7 +541,7 @@
         <v>972.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>39722</v>
       </c>
@@ -534,7 +549,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>39753</v>
       </c>
@@ -542,7 +557,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>39783</v>
       </c>
@@ -550,7 +565,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>39814</v>
       </c>
@@ -558,7 +573,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>39845</v>
       </c>
@@ -566,7 +581,7 @@
         <v>912.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>39873</v>
       </c>
@@ -574,7 +589,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>39904</v>
       </c>
@@ -582,7 +597,7 @@
         <v>757.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>39934</v>
       </c>
@@ -590,7 +605,7 @@
         <v>757.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>39965</v>
       </c>
@@ -598,7 +613,7 @@
         <v>757.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>39995</v>
       </c>
@@ -606,7 +621,7 @@
         <v>757.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>40026</v>
       </c>
@@ -614,7 +629,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>40057</v>
       </c>
@@ -622,7 +637,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>40087</v>
       </c>
@@ -630,7 +645,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>40118</v>
       </c>
@@ -638,7 +653,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>40148</v>
       </c>
@@ -646,7 +661,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>40179</v>
       </c>
@@ -654,7 +669,7 @@
         <v>402.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>40210</v>
       </c>
@@ -662,7 +677,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>40238</v>
       </c>
@@ -670,7 +685,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>40269</v>
       </c>
@@ -678,7 +693,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>40299</v>
       </c>
@@ -686,7 +701,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>40330</v>
       </c>
@@ -694,7 +709,7 @@
         <v>398.75</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>40360</v>
       </c>
@@ -702,7 +717,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>40391</v>
       </c>
@@ -710,7 +725,7 @@
         <v>392.5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>40422</v>
       </c>
@@ -718,7 +733,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>40452</v>
       </c>
@@ -726,7 +741,7 @@
         <v>396.25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>40483</v>
       </c>
@@ -734,7 +749,7 @@
         <v>407.5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>40513</v>
       </c>
@@ -742,7 +757,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>40544</v>
       </c>
@@ -750,7 +765,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>40575</v>
       </c>
@@ -758,7 +773,7 @@
         <v>450.625</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>40603</v>
       </c>
@@ -766,7 +781,7 @@
         <v>467.5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40634</v>
       </c>
@@ -774,7 +789,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>40664</v>
       </c>
@@ -782,7 +797,7 @@
         <v>502.5</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>40695</v>
       </c>
@@ -790,7 +805,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>40725</v>
       </c>
@@ -798,7 +813,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>40756</v>
       </c>
@@ -806,7 +821,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>40787</v>
       </c>
@@ -814,7 +829,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>40817</v>
       </c>
@@ -822,7 +837,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>40848</v>
       </c>
@@ -830,7 +845,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>40878</v>
       </c>
@@ -838,7 +853,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>40909</v>
       </c>
@@ -846,7 +861,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>40940</v>
       </c>
@@ -854,7 +869,7 @@
         <v>546.25</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>40969</v>
       </c>
@@ -862,7 +877,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>41000</v>
       </c>
@@ -870,7 +885,7 @@
         <v>518.75</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>41030</v>
       </c>
@@ -878,7 +893,7 @@
         <v>517.5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>41061</v>
       </c>
@@ -886,7 +901,7 @@
         <v>523.125</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>41091</v>
       </c>
@@ -894,7 +909,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>41122</v>
       </c>
@@ -902,7 +917,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>41153</v>
       </c>
@@ -910,7 +925,7 @@
         <v>506.25</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>41183</v>
       </c>
@@ -918,7 +933,7 @@
         <v>492.5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>41214</v>
       </c>
@@ -926,7 +941,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>41244</v>
       </c>
@@ -934,7 +949,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>41275</v>
       </c>
@@ -942,7 +957,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>41306</v>
       </c>
@@ -950,7 +965,7 @@
         <v>437.5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>41334</v>
       </c>
@@ -958,7 +973,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>41365</v>
       </c>
@@ -966,7 +981,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>41395</v>
       </c>
@@ -974,7 +989,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>41426</v>
       </c>
@@ -982,7 +997,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>41456</v>
       </c>
@@ -990,7 +1005,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>41487</v>
       </c>
@@ -998,7 +1013,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>41518</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>41548</v>
       </c>
@@ -1014,7 +1029,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>41579</v>
       </c>
@@ -1022,7 +1037,7 @@
         <v>334.375</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>41609</v>
       </c>
@@ -1030,7 +1045,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>41640</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>41671</v>
       </c>
@@ -1046,7 +1061,7 @@
         <v>328.125</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>41699</v>
       </c>
@@ -1054,7 +1069,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>41730</v>
       </c>
@@ -1062,7 +1077,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>41760</v>
       </c>
@@ -1070,7 +1085,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>41791</v>
       </c>
@@ -1078,7 +1093,7 @@
         <v>345.625</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>41821</v>
       </c>
@@ -1086,7 +1101,7 @@
         <v>348.5</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>41852</v>
       </c>
@@ -1094,7 +1109,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>41883</v>
       </c>
@@ -1102,7 +1117,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>41913</v>
       </c>
@@ -1110,7 +1125,7 @@
         <v>373.5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>41944</v>
       </c>
@@ -1118,7 +1133,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>41974</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>370.625</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>42005</v>
       </c>
@@ -1134,7 +1149,7 @@
         <v>370.5</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>42036</v>
       </c>
@@ -1142,7 +1157,7 @@
         <v>363.75</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>42064</v>
       </c>
@@ -1150,7 +1165,7 @@
         <v>347.5</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>42095</v>
       </c>
@@ -1158,7 +1173,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>42125</v>
       </c>
@@ -1166,7 +1181,7 @@
         <v>334.375</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>42156</v>
       </c>
@@ -1174,7 +1189,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>42186</v>
       </c>
@@ -1182,7 +1197,7 @@
         <v>328.5</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>42217</v>
       </c>
@@ -1190,7 +1205,7 @@
         <v>313.75</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>42248</v>
       </c>
@@ -1198,7 +1213,7 @@
         <v>305.625</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>42278</v>
       </c>
@@ -1206,7 +1221,7 @@
         <v>297.5</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>42309</v>
       </c>
@@ -1214,7 +1229,7 @@
         <v>293.125</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>42339</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>42370</v>
       </c>
@@ -1230,7 +1245,7 @@
         <v>258.75</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>42401</v>
       </c>
@@ -1238,7 +1253,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>42430</v>
       </c>
@@ -1246,7 +1261,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>42461</v>
       </c>
@@ -1254,7 +1269,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>42491</v>
       </c>
@@ -1262,7 +1277,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>42522</v>
       </c>
@@ -1270,7 +1285,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>42552</v>
       </c>
@@ -1278,7 +1293,7 @@
         <v>218.75</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>42583</v>
       </c>
@@ -1286,7 +1301,7 @@
         <v>231.25</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>42614</v>
       </c>
@@ -1294,7 +1309,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>42644</v>
       </c>
@@ -1302,7 +1317,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>42675</v>
       </c>
@@ -1310,7 +1325,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>42705</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>42736</v>
       </c>
@@ -1326,7 +1341,7 @@
         <v>238.75</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>42767</v>
       </c>
@@ -1334,7 +1349,7 @@
         <v>245.625</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>42795</v>
       </c>
@@ -1342,7 +1357,7 @@
         <v>249.5</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>42826</v>
       </c>
@@ -1350,7 +1365,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>42856</v>
       </c>
@@ -1358,7 +1373,7 @@
         <v>260.625</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>42887</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>42917</v>
       </c>
@@ -1374,7 +1389,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>42948</v>
       </c>
@@ -1382,7 +1397,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>42979</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>43009</v>
       </c>
@@ -1398,7 +1413,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>43040</v>
       </c>
@@ -1406,7 +1421,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>43070</v>
       </c>
@@ -1414,7 +1429,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>43101</v>
       </c>
@@ -1422,7 +1437,7 @@
         <v>287.5</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>43132</v>
       </c>
@@ -1430,7 +1445,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>43160</v>
       </c>
@@ -1438,7 +1453,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>43191</v>
       </c>
@@ -1446,7 +1461,7 @@
         <v>303.125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>43221</v>
       </c>
@@ -1454,7 +1469,7 @@
         <v>309.2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>43252</v>
       </c>
@@ -1462,7 +1477,7 @@
         <v>312.75</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>43282</v>
       </c>
@@ -1470,7 +1485,7 @@
         <v>322.5</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>43313</v>
       </c>
@@ -1478,7 +1493,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>43344</v>
       </c>
@@ -1486,7 +1501,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>43374</v>
       </c>
@@ -1494,7 +1509,7 @@
         <v>348.75</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>43405</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>350.5</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>43435</v>
       </c>
@@ -1510,7 +1525,7 @@
         <v>352.5</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>43466</v>
       </c>
@@ -1518,7 +1533,7 @@
         <v>352.5</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>43497</v>
       </c>
@@ -1526,7 +1541,7 @@
         <v>351.875</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>43525</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>43556</v>
       </c>
@@ -1542,7 +1557,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>43586</v>
       </c>
@@ -1550,7 +1565,7 @@
         <v>347.5</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>43617</v>
       </c>
@@ -1558,7 +1573,7 @@
         <v>341.25</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>43647</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>43678</v>
       </c>
@@ -1574,7 +1589,7 @@
         <v>328.5</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>43709</v>
       </c>
@@ -1582,7 +1597,7 @@
         <v>315.625</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>43739</v>
       </c>
@@ -1590,7 +1605,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>43770</v>
       </c>
@@ -1598,7 +1613,7 @@
         <v>291.25</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>43800</v>
       </c>
@@ -1606,7 +1621,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>43831</v>
       </c>
@@ -1614,7 +1629,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>43862</v>
       </c>
@@ -1622,7 +1637,7 @@
         <v>241.5</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>43891</v>
       </c>
@@ -1630,7 +1645,7 @@
         <v>229.375</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>43922</v>
       </c>
@@ -1638,7 +1653,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>43952</v>
       </c>
@@ -1646,7 +1661,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>43983</v>
       </c>
@@ -1654,7 +1669,7 @@
         <v>228.125</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>44013</v>
       </c>
@@ -1662,7 +1677,7 @@
         <v>235.5</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="2">
         <v>44044</v>
       </c>
@@ -1670,7 +1685,7 @@
         <v>238.125</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>44075</v>
       </c>
@@ -1678,7 +1693,7 @@
         <v>244.375</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>44105</v>
       </c>
@@ -1686,7 +1701,7 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="2">
         <v>44136</v>
       </c>
@@ -1694,7 +1709,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="2">
         <v>44166</v>
       </c>
@@ -1702,7 +1717,7 @@
         <v>246.25</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="2">
         <v>44197</v>
       </c>
@@ -1710,7 +1725,7 @@
         <v>251.875</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="2">
         <v>44228</v>
       </c>
@@ -1718,7 +1733,7 @@
         <v>285.625</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="2">
         <v>44256</v>
       </c>
@@ -1726,7 +1741,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="2">
         <v>44287</v>
       </c>
@@ -1734,7 +1749,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="2">
         <v>44317</v>
       </c>
@@ -1742,7 +1757,7 @@
         <v>373.125</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="2">
         <v>44348</v>
       </c>
@@ -1750,7 +1765,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>44378</v>
       </c>
@@ -1758,7 +1773,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>44409</v>
       </c>
@@ -1766,7 +1781,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="2">
         <v>44440</v>
       </c>
@@ -1774,7 +1789,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="2">
         <v>44470</v>
       </c>
@@ -1782,7 +1797,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="2">
         <v>44501</v>
       </c>
@@ -1790,7 +1805,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="2">
         <v>44531</v>
       </c>
@@ -1798,7 +1813,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="2">
         <v>44562</v>
       </c>
@@ -1806,7 +1821,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="2">
         <v>44593</v>
       </c>
@@ -1814,7 +1829,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="2">
         <v>44621</v>
       </c>
@@ -1822,7 +1837,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="2">
         <v>44652</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>44682</v>
       </c>
@@ -1838,7 +1853,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="2">
         <v>44713</v>
       </c>
@@ -1846,12 +1861,76 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="3">
         <v>44743</v>
       </c>
       <c r="B176">
         <v>969</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B177">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A178" s="3">
+        <v>44805</v>
+      </c>
+      <c r="B178" s="4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A179" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B179" s="4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A180" s="3">
+        <v>44866</v>
+      </c>
+      <c r="B180" s="4">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A181" s="2">
+        <v>44896</v>
+      </c>
+      <c r="B181" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A182" s="3">
+        <v>44927</v>
+      </c>
+      <c r="B182" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A183" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B183" s="4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A184" s="3">
+        <v>44986</v>
+      </c>
+      <c r="B184" s="4">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Canpotex Data feed updated for 2023 Manual forecast
</commit_message>
<xml_diff>
--- a/DataFeeds/BrazilCFR.xlsx
+++ b/DataFeeds/BrazilCFR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meesam/Sandbox/Nutrien/Canpotex/DataFeeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B2A91A-4254-9943-9188-623D66340B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9A1892-5AA2-1343-AF00-9371948178DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="820" windowWidth="25900" windowHeight="18380" xr2:uid="{8A4C0F15-AD97-40A7-9824-0E46FEA19653}"/>
+    <workbookView xWindow="12760" yWindow="740" windowWidth="25900" windowHeight="18380" xr2:uid="{8A4C0F15-AD97-40A7-9824-0E46FEA19653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0731233C-0420-4FB5-BC73-AB9A7C487093}">
   <dimension ref="A1:B193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1798,7 +1798,7 @@
         <v>44593</v>
       </c>
       <c r="B171">
-        <v>781</v>
+        <v>781.25</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
@@ -1814,7 +1814,7 @@
         <v>44652</v>
       </c>
       <c r="B173">
-        <v>1174</v>
+        <v>1173.75</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -1838,7 +1838,7 @@
         <v>44743</v>
       </c>
       <c r="B176">
-        <v>969</v>
+        <v>968.75</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
@@ -1854,7 +1854,7 @@
         <v>44805</v>
       </c>
       <c r="B178">
-        <v>750</v>
+        <v>731</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -1862,7 +1862,7 @@
         <v>44835</v>
       </c>
       <c r="B179">
-        <v>650</v>
+        <v>629</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -1870,7 +1870,7 @@
         <v>44866</v>
       </c>
       <c r="B180">
-        <v>675</v>
+        <v>564</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -1878,7 +1878,7 @@
         <v>44896</v>
       </c>
       <c r="B181">
-        <v>700</v>
+        <v>516</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>